<commit_message>
penAndPaper complete, just need to finish report
</commit_message>
<xml_diff>
--- a/H04/penAndPaper/penAndPaper.xlsx
+++ b/H04/penAndPaper/penAndPaper.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\Uni\3Ano\1Semestre\Aprendizagem\homeworks\H04\penAndPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5559203E-1107-4AAA-98BE-8DE84C01670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157A32E2-2C46-405E-A8E8-6468364DAC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" activeTab="1" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
+    <workbookView xWindow="3777" yWindow="530" windowWidth="19562" windowHeight="10352" activeTab="1" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>y1</t>
   </si>
@@ -129,6 +130,39 @@
   </si>
   <si>
     <t>iii) new cov matrix</t>
+  </si>
+  <si>
+    <t>3) fazer sketch</t>
+  </si>
+  <si>
+    <t>a(X)</t>
+  </si>
+  <si>
+    <t>X = x1</t>
+  </si>
+  <si>
+    <t>X = x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X = x3 </t>
+  </si>
+  <si>
+    <t>X = x4</t>
+  </si>
+  <si>
+    <t>b(X)</t>
+  </si>
+  <si>
+    <t>S(X)</t>
+  </si>
+  <si>
+    <t>X = c1</t>
+  </si>
+  <si>
+    <t>X = c2</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -136,10 +170,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="198" formatCode="0.00000%"/>
-    <numFmt numFmtId="199" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.00000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,16 +188,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -200,12 +259,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,7 +292,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -228,28 +324,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -654,8 +738,8 @@
       <xdr:rowOff>172528</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="224420" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -697,6 +781,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -739,7 +824,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -806,8 +891,8 @@
       <xdr:rowOff>181154</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="226088" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -849,6 +934,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -891,7 +977,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -958,8 +1044,8 @@
       <xdr:rowOff>17253</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="171265" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1001,6 +1087,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1043,7 +1130,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1107,8 +1194,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="174535" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -1150,6 +1237,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1192,7 +1280,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -1548,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7EE557-5011-4EFA-8AC3-434123C8EEDB}">
-  <dimension ref="B3:P43"/>
+  <dimension ref="B3:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1599,10 +1687,10 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="23">
         <v>0.7</v>
       </c>
       <c r="I5" s="2">
@@ -1625,8 +1713,8 @@
       <c r="D6">
         <v>-4</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="3">
         <v>4</v>
       </c>
@@ -1647,10 +1735,10 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="25">
         <v>2</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="25">
         <v>0.3</v>
       </c>
       <c r="I7" s="5">
@@ -1673,8 +1761,8 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="3">
         <v>-4</v>
       </c>
@@ -1691,32 +1779,32 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="6" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="6" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="6" t="s">
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1725,16 +1813,16 @@
       <c r="D14" s="2">
         <v>0.15915494309189501</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="10">
         <v>2.2390899578253199E-17</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1743,48 +1831,48 @@
       <c r="L14" s="2">
         <v>2.3927977920047E-4</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="N14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="10">
         <v>7.2256232377243201E-6</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="8">
         <v>9.4387795134662607E-10</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="3">
         <v>7.9577471545947603E-2</v>
       </c>
-      <c r="J15" s="8"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="8">
         <v>9.8206401731987101E-6</v>
       </c>
-      <c r="N15" s="8"/>
+      <c r="N15" s="24"/>
       <c r="O15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="13">
+      <c r="P15" s="8">
         <v>2.8136605178593099E-6</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1794,17 +1882,17 @@
         <f>H5*D14</f>
         <v>0.1114084601643265</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="9">
         <f>H5*H14</f>
         <v>1.5673629704777237E-17</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="25" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1814,27 +1902,27 @@
         <f>L14*H5</f>
         <v>1.67495845440329E-4</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="25" t="s">
         <v>12</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16" s="9">
         <f>P14*H5</f>
         <v>5.0579362664070234E-6</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="8">
         <f>H7*D15</f>
         <v>2.8316338540398779E-10</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1842,166 +1930,166 @@
         <f>H15*H7</f>
         <v>2.3873241463784282E-2</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="8">
         <f>L15*H7</f>
         <v>2.9461920519596129E-6</v>
       </c>
-      <c r="N17" s="8"/>
+      <c r="N17" s="24"/>
       <c r="O17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="13">
+      <c r="P17" s="8">
         <f>P15*H7</f>
         <v>8.4409815535779294E-7</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="26">
         <f>D16+D17</f>
         <v>0.11140846044748988</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="F18" s="10" t="s">
+      <c r="D18" s="22"/>
+      <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="26">
         <f>H16+H17</f>
         <v>2.3873241463784299E-2</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="J18" s="10" t="s">
+      <c r="H18" s="22"/>
+      <c r="J18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="26">
         <f>L16+L17</f>
         <v>1.704420374922886E-4</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="N18" s="10" t="s">
+      <c r="L18" s="22"/>
+      <c r="N18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="26">
         <f>P16+P17</f>
         <v>5.9020344217648163E-6</v>
       </c>
-      <c r="P18" s="11"/>
+      <c r="P18" s="22"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="11">
         <f>D16/C18</f>
         <v>0.99999999745833146</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="11">
         <f>H16/G18</f>
         <v>6.5653546580819908E-16</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="25" t="s">
         <v>14</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19" s="11">
         <f>L16/K18</f>
         <v>0.98271440487741823</v>
       </c>
-      <c r="N19" s="9" t="s">
+      <c r="N19" s="25" t="s">
         <v>14</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P19" s="17">
+      <c r="P19" s="11">
         <f>P16/O18</f>
         <v>0.85698183117248028</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="12">
         <f>D17/C18</f>
         <v>2.5416685973993073E-9</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="12">
         <f>H17/G18</f>
         <v>0.99999999999999922</v>
       </c>
-      <c r="J20" s="8"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="12">
         <f>L17/K18</f>
         <v>1.7285595122581827E-2</v>
       </c>
-      <c r="N20" s="8"/>
+      <c r="N20" s="24"/>
       <c r="O20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="18">
+      <c r="P20" s="12">
         <f>P17/O18</f>
         <v>0.14301816882751966</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="11" t="str">
+      <c r="C21" s="22" t="str">
         <f>IF(D19&gt;D20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="F21" s="10" t="s">
+      <c r="D21" s="22"/>
+      <c r="F21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="11" t="str">
+      <c r="G21" s="22" t="str">
         <f>IF(H19&gt;H20, "c1", "c2")</f>
         <v>c2</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="J21" s="10" t="s">
+      <c r="H21" s="22"/>
+      <c r="J21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="11" t="str">
+      <c r="K21" s="22" t="str">
         <f>IF(L19&gt;L20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="L21" s="11"/>
-      <c r="N21" s="10" t="s">
+      <c r="L21" s="22"/>
+      <c r="N21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="11" t="str">
+      <c r="O21" s="22" t="str">
         <f>IF(P19&gt;P20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="P21" s="11"/>
+      <c r="P21" s="22"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2028,11 +2116,11 @@
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="19">
+      <c r="B27" s="13">
         <f>D19</f>
         <v>0.99999999745833146</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="13">
         <f>D20</f>
         <v>2.5416685973993073E-9</v>
       </c>
@@ -2044,25 +2132,25 @@
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="19">
+      <c r="B28" s="13">
         <f>H19</f>
         <v>6.5653546580819908E-16</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="13">
         <f>H20</f>
         <v>0.99999999999999922</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="16">
         <f>B31/(D31+B31)</f>
         <v>0.70992405837705763</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="17">
         <f>D31/(D31+B31)</f>
         <v>0.29007594162294231</v>
       </c>
@@ -2090,11 +2178,11 @@
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="19">
+      <c r="B29" s="13">
         <f>L19</f>
         <v>0.98271440487741823</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="13">
         <f>L20</f>
         <v>1.7285595122581827E-2</v>
       </c>
@@ -2118,21 +2206,21 @@
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="20">
+      <c r="B30" s="14">
         <f>P19</f>
         <v>0.85698183117248028</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="14">
         <f>P20</f>
         <v>0.14301816882751966</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="21">
+      <c r="B31" s="15">
         <f>SUM(B27:B30)</f>
         <v>2.8396962335082305</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="15">
         <f>SUM(D27:D30)</f>
         <v>1.1603037664917693</v>
       </c>
@@ -2140,12 +2228,12 @@
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M33">
         <f>(C5 - J28)^2</f>
         <v>0.18889172069456414</v>
@@ -2163,7 +2251,7 @@
         <v>17.681308905409278</v>
       </c>
     </row>
-    <row r="34" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M34" s="3">
         <f>(C5 - J28)*(D5 - J29)</f>
         <v>0.82545551712130794</v>
@@ -2181,13 +2269,13 @@
         <v>55.020465609608181</v>
       </c>
     </row>
-    <row r="35" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-    </row>
-    <row r="36" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M36">
         <f>(C6 - J28)^2</f>
         <v>6.5811912116244917</v>
@@ -2205,7 +2293,7 @@
         <v>0.35894439793574856</v>
       </c>
     </row>
-    <row r="37" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M37" s="3">
         <f>(C6 - J28)*(D6 - J29)</f>
         <v>15.650704882105138</v>
@@ -2223,13 +2311,13 @@
         <v>0.33921521149477174</v>
       </c>
     </row>
-    <row r="38" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-    </row>
-    <row r="39" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M39">
         <f>(C6 - J28)^2</f>
         <v>6.5811912116244917</v>
@@ -2247,7 +2335,7 @@
         <v>-3.3388330586938033</v>
       </c>
     </row>
-    <row r="40" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M40" s="3">
         <f>(C7 - J28)*(D7 - J29)</f>
         <v>0.25840539117521122</v>
@@ -2265,13 +2353,13 @@
         <v>29.350153010079826</v>
       </c>
     </row>
-    <row r="41" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-    </row>
-    <row r="42" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M42">
         <f>(C8 - J28)^2</f>
         <v>5.9273587267412795</v>
@@ -2289,7 +2377,7 @@
         <v>14.981650176259819</v>
       </c>
     </row>
-    <row r="43" spans="13:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M43" s="3">
         <f>(C8 - J28)*(D8 - J29)</f>
         <v>-5.1144670736435804</v>
@@ -2307,27 +2395,41 @@
         <v>11.679840410551474</v>
       </c>
     </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N44" s="19"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B48" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="J19:J20"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B20"/>
@@ -2337,16 +2439,25 @@
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M41:N41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2356,9 +2467,153 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2303F90-97BD-41BC-954F-99D4AF5EB548}">
+  <dimension ref="B4:R6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="G4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="L4" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4.0388436152317801</v>
+      </c>
+      <c r="C6">
+        <v>4.49535804129924</v>
+      </c>
+      <c r="D6">
+        <v>4.9286503810670403</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>8.5440037453175304</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>6.4031242374328396</v>
+      </c>
+      <c r="J6">
+        <v>6.9823759942501198</v>
+      </c>
+      <c r="L6">
+        <f xml:space="preserve"> 1 - B6/G6</f>
+        <v>0.527289109927505</v>
+      </c>
+      <c r="M6">
+        <f xml:space="preserve"> 1 - C6/H6</f>
+        <v>0.25077365978346</v>
+      </c>
+      <c r="N6">
+        <f xml:space="preserve"> 1 - D6/I6</f>
+        <v>0.2302741289550474</v>
+      </c>
+      <c r="O6">
+        <f xml:space="preserve"> 1 - E6/J6</f>
+        <v>0.85678227571481613</v>
+      </c>
+      <c r="P6">
+        <f>(L6 + N6 + O6)/3</f>
+        <v>0.53811517153245614</v>
+      </c>
+      <c r="Q6">
+        <f>M6</f>
+        <v>0.25077365978346</v>
+      </c>
+      <c r="R6">
+        <f>(P6 + Q6)/2</f>
+        <v>0.39444441565795807</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="L4:R4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FE25E0-FDB5-4B21-A78E-0E7A9C27B497}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
stated doing first question from penAndPaper [report]
</commit_message>
<xml_diff>
--- a/H04/penAndPaper/penAndPaper.xlsx
+++ b/H04/penAndPaper/penAndPaper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\Uni\3Ano\1Semestre\Aprendizagem\homeworks\H04\penAndPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157A32E2-2C46-405E-A8E8-6468364DAC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5B3E87-E19B-4AFA-A11A-93C63520206A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3777" yWindow="530" windowWidth="19562" windowHeight="10352" activeTab="1" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -309,12 +309,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,7 +318,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1638,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7EE557-5011-4EFA-8AC3-434123C8EEDB}">
   <dimension ref="B3:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1687,10 +1687,10 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="21">
         <v>1</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="21">
         <v>0.7</v>
       </c>
       <c r="I5" s="2">
@@ -1713,8 +1713,8 @@
       <c r="D6">
         <v>-4</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="3">
         <v>4</v>
       </c>
@@ -1735,10 +1735,10 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <v>2</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="23">
         <v>0.3</v>
       </c>
       <c r="I7" s="5">
@@ -1761,8 +1761,8 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="3">
         <v>-4</v>
       </c>
@@ -1779,32 +1779,32 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="21" t="s">
+      <c r="N13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1813,7 +1813,7 @@
       <c r="D14" s="2">
         <v>0.15915494309189501</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1822,7 +1822,7 @@
       <c r="H14" s="10">
         <v>2.2390899578253199E-17</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1831,7 +1831,7 @@
       <c r="L14" s="2">
         <v>2.3927977920047E-4</v>
       </c>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -1842,28 +1842,28 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="8">
         <v>9.4387795134662607E-10</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="3">
         <v>7.9577471545947603E-2</v>
       </c>
-      <c r="J15" s="24"/>
+      <c r="J15" s="22"/>
       <c r="K15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="L15" s="8">
         <v>9.8206401731987101E-6</v>
       </c>
-      <c r="N15" s="24"/>
+      <c r="N15" s="22"/>
       <c r="O15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1882,7 +1882,7 @@
         <f>H5*D14</f>
         <v>0.1114084601643265</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1892,7 +1892,7 @@
         <f>H5*H14</f>
         <v>1.5673629704777237E-17</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1902,7 +1902,7 @@
         <f>L14*H5</f>
         <v>1.67495845440329E-4</v>
       </c>
-      <c r="N16" s="25" t="s">
+      <c r="N16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="O16" s="2" t="s">
@@ -1914,7 +1914,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1922,7 +1922,7 @@
         <f>H7*D15</f>
         <v>2.8316338540398779E-10</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="22"/>
       <c r="G17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1930,7 @@
         <f>H15*H7</f>
         <v>2.3873241463784282E-2</v>
       </c>
-      <c r="J17" s="24"/>
+      <c r="J17" s="22"/>
       <c r="K17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1938,7 +1938,7 @@
         <f>L15*H7</f>
         <v>2.9461920519596129E-6</v>
       </c>
-      <c r="N17" s="24"/>
+      <c r="N17" s="22"/>
       <c r="O17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1951,38 +1951,38 @@
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="25">
         <f>D16+D17</f>
         <v>0.11140846044748988</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="26"/>
       <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="25">
         <f>H16+H17</f>
         <v>2.3873241463784299E-2</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="26"/>
       <c r="J18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="25">
         <f>L16+L17</f>
         <v>1.704420374922886E-4</v>
       </c>
-      <c r="L18" s="22"/>
+      <c r="L18" s="26"/>
       <c r="N18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="25">
         <f>P16+P17</f>
         <v>5.9020344217648163E-6</v>
       </c>
-      <c r="P18" s="22"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1992,7 +1992,7 @@
         <f>D16/C18</f>
         <v>0.99999999745833146</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -2002,7 +2002,7 @@
         <f>H16/G18</f>
         <v>6.5653546580819908E-16</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -2012,7 +2012,7 @@
         <f>L16/K18</f>
         <v>0.98271440487741823</v>
       </c>
-      <c r="N19" s="25" t="s">
+      <c r="N19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2032,7 +2032,7 @@
         <f>D17/C18</f>
         <v>2.5416685973993073E-9</v>
       </c>
-      <c r="F20" s="24"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2040,7 +2040,7 @@
         <f>H17/G18</f>
         <v>0.99999999999999922</v>
       </c>
-      <c r="J20" s="24"/>
+      <c r="J20" s="22"/>
       <c r="K20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2048,7 +2048,7 @@
         <f>L17/K18</f>
         <v>1.7285595122581827E-2</v>
       </c>
-      <c r="N20" s="24"/>
+      <c r="N20" s="22"/>
       <c r="O20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2061,35 +2061,35 @@
       <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="22" t="str">
+      <c r="C21" s="26" t="str">
         <f>IF(D19&gt;D20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="26"/>
       <c r="F21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="22" t="str">
+      <c r="G21" s="26" t="str">
         <f>IF(H19&gt;H20, "c1", "c2")</f>
         <v>c2</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="26"/>
       <c r="J21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="22" t="str">
+      <c r="K21" s="26" t="str">
         <f>IF(L19&gt;L20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="L21" s="22"/>
+      <c r="L21" s="26"/>
       <c r="N21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="22" t="str">
+      <c r="O21" s="26" t="str">
         <f>IF(P19&gt;P20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="P21" s="22"/>
+      <c r="P21" s="26"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2132,10 +2132,10 @@
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
@@ -2228,10 +2228,10 @@
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M33">
@@ -2270,10 +2270,10 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M36">
@@ -2312,10 +2312,10 @@
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="21"/>
-      <c r="P38" s="21"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M39">
@@ -2354,10 +2354,10 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M42">
@@ -2420,16 +2420,25 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="N19:N20"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B20"/>
@@ -2439,25 +2448,16 @@
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2469,25 +2469,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2303F90-97BD-41BC-954F-99D4AF5EB548}">
   <dimension ref="B4:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="G4" s="21" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="G4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="L4" s="27" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
word = worst shit ever made
</commit_message>
<xml_diff>
--- a/H04/penAndPaper/penAndPaper.xlsx
+++ b/H04/penAndPaper/penAndPaper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\Uni\3Ano\1Semestre\Aprendizagem\homeworks\H04\penAndPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5B3E87-E19B-4AFA-A11A-93C63520206A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CA6ACA-8C02-4BDF-8DD7-1623A57C673F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
+    <workbookView xWindow="3777" yWindow="530" windowWidth="19562" windowHeight="10352" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="172" formatCode="0.000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -281,7 +285,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,12 +307,17 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -318,18 +327,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1638,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7EE557-5011-4EFA-8AC3-434123C8EEDB}">
   <dimension ref="B3:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K29" sqref="K28:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1687,10 +1699,10 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="22">
         <v>1</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="22">
         <v>0.7</v>
       </c>
       <c r="I5" s="2">
@@ -1713,8 +1725,8 @@
       <c r="D6">
         <v>-4</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="3">
         <v>4</v>
       </c>
@@ -1735,10 +1747,10 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="24">
         <v>2</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="24">
         <v>0.3</v>
       </c>
       <c r="I7" s="5">
@@ -1761,8 +1773,8 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="3">
         <v>-4</v>
       </c>
@@ -1779,32 +1791,32 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="24" t="s">
+      <c r="N13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1813,7 +1825,7 @@
       <c r="D14" s="2">
         <v>0.15915494309189501</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="22" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1822,7 +1834,7 @@
       <c r="H14" s="10">
         <v>2.2390899578253199E-17</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="22" t="s">
         <v>9</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1831,7 +1843,7 @@
       <c r="L14" s="2">
         <v>2.3927977920047E-4</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="N14" s="22" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -1842,28 +1854,28 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="8">
         <v>9.4387795134662607E-10</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="3">
         <v>7.9577471545947603E-2</v>
       </c>
-      <c r="J15" s="22"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="L15" s="8">
         <v>9.8206401731987101E-6</v>
       </c>
-      <c r="N15" s="22"/>
+      <c r="N15" s="23"/>
       <c r="O15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1872,7 +1884,7 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1882,7 +1894,7 @@
         <f>H5*D14</f>
         <v>0.1114084601643265</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1892,7 +1904,7 @@
         <f>H5*H14</f>
         <v>1.5673629704777237E-17</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1902,7 +1914,7 @@
         <f>L14*H5</f>
         <v>1.67495845440329E-4</v>
       </c>
-      <c r="N16" s="23" t="s">
+      <c r="N16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="O16" s="2" t="s">
@@ -1914,15 +1926,15 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="26">
         <f>H7*D15</f>
         <v>2.8316338540398779E-10</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1942,7 @@
         <f>H15*H7</f>
         <v>2.3873241463784282E-2</v>
       </c>
-      <c r="J17" s="22"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1938,7 +1950,7 @@
         <f>L15*H7</f>
         <v>2.9461920519596129E-6</v>
       </c>
-      <c r="N17" s="22"/>
+      <c r="N17" s="23"/>
       <c r="O17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1951,38 +1963,38 @@
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="28">
         <f>D16+D17</f>
         <v>0.11140846044748988</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="28"/>
       <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="27">
         <f>H16+H17</f>
         <v>2.3873241463784299E-2</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="27"/>
       <c r="J18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="28">
         <f>L16+L17</f>
         <v>1.704420374922886E-4</v>
       </c>
-      <c r="L18" s="26"/>
+      <c r="L18" s="28"/>
       <c r="N18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="28">
         <f>P16+P17</f>
         <v>5.9020344217648163E-6</v>
       </c>
-      <c r="P18" s="26"/>
+      <c r="P18" s="28"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1992,7 +2004,7 @@
         <f>D16/C18</f>
         <v>0.99999999745833146</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="24" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -2002,29 +2014,29 @@
         <f>H16/G18</f>
         <v>6.5653546580819908E-16</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="24" t="s">
         <v>14</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="29">
         <f>L16/K18</f>
         <v>0.98271440487741823</v>
       </c>
-      <c r="N19" s="23" t="s">
+      <c r="N19" s="24" t="s">
         <v>14</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P19" s="11">
+      <c r="P19" s="31">
         <f>P16/O18</f>
         <v>0.85698183117248028</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2032,7 +2044,7 @@
         <f>D17/C18</f>
         <v>2.5416685973993073E-9</v>
       </c>
-      <c r="F20" s="22"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2040,19 +2052,19 @@
         <f>H17/G18</f>
         <v>0.99999999999999922</v>
       </c>
-      <c r="J20" s="22"/>
+      <c r="J20" s="23"/>
       <c r="K20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="30">
         <f>L17/K18</f>
         <v>1.7285595122581827E-2</v>
       </c>
-      <c r="N20" s="22"/>
+      <c r="N20" s="23"/>
       <c r="O20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="30">
         <f>P17/O18</f>
         <v>0.14301816882751966</v>
       </c>
@@ -2061,35 +2073,35 @@
       <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="26" t="str">
+      <c r="C21" s="21" t="str">
         <f>IF(D19&gt;D20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="21"/>
       <c r="F21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="26" t="str">
+      <c r="G21" s="21" t="str">
         <f>IF(H19&gt;H20, "c1", "c2")</f>
         <v>c2</v>
       </c>
-      <c r="H21" s="26"/>
+      <c r="H21" s="21"/>
       <c r="J21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="26" t="str">
+      <c r="K21" s="21" t="str">
         <f>IF(L19&gt;L20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="L21" s="26"/>
+      <c r="L21" s="21"/>
       <c r="N21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="26" t="str">
+      <c r="O21" s="21" t="str">
         <f>IF(P19&gt;P20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="P21" s="26"/>
+      <c r="P21" s="21"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2132,10 +2144,10 @@
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
@@ -2146,11 +2158,11 @@
         <f>H20</f>
         <v>0.99999999999999922</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="15">
         <f>B31/(D31+B31)</f>
         <v>0.70992405837705763</v>
       </c>
-      <c r="H28" s="17">
+      <c r="H28" s="16">
         <f>D31/(D31+B31)</f>
         <v>0.29007594162294231</v>
       </c>
@@ -2216,11 +2228,11 @@
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="15">
+      <c r="B31" s="32">
         <f>SUM(B27:B30)</f>
         <v>2.8396962335082305</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="33">
         <f>SUM(D27:D30)</f>
         <v>1.1603037664917693</v>
       </c>
@@ -2228,10 +2240,10 @@
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M33">
@@ -2270,10 +2282,10 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M36">
@@ -2312,10 +2324,10 @@
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M38" s="24"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M39">
@@ -2354,10 +2366,10 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M42">
@@ -2396,49 +2408,40 @@
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="N44" s="19"/>
+      <c r="N44" s="18"/>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="J19:J20"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B20"/>
@@ -2448,16 +2451,25 @@
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M41:N41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2476,51 +2488,51 @@
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="G4" s="24" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="G4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="L4" s="27" t="s">
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="L4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="19" t="s">
         <v>29</v>
       </c>
       <c r="L5" s="3" t="s">

</xml_diff>

<commit_message>
some error fixes to penAndPaper 2
</commit_message>
<xml_diff>
--- a/H04/penAndPaper/penAndPaper.xlsx
+++ b/H04/penAndPaper/penAndPaper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\Uni\3Ano\1Semestre\Aprendizagem\homeworks\H04\penAndPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CA6ACA-8C02-4BDF-8DD7-1623A57C673F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D157C00C-4256-4CDF-B7C4-4A934DC01974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3777" yWindow="530" windowWidth="19562" windowHeight="10352" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" activeTab="1" xr2:uid="{D8C3BDBA-A6B4-48EB-B35A-30EBE73BA983}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -173,9 +173,9 @@
     <numFmt numFmtId="164" formatCode="0.00000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
-    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="169" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="172" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -312,12 +312,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -327,21 +327,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1650,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7EE557-5011-4EFA-8AC3-434123C8EEDB}">
   <dimension ref="B3:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K29" sqref="K28:K29"/>
     </sheetView>
   </sheetViews>
@@ -1699,10 +1699,10 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="26">
         <v>1</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="26">
         <v>0.7</v>
       </c>
       <c r="I5" s="2">
@@ -1725,8 +1725,8 @@
       <c r="D6">
         <v>-4</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="3">
         <v>4</v>
       </c>
@@ -1747,10 +1747,10 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="28">
         <v>2</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="28">
         <v>0.3</v>
       </c>
       <c r="I7" s="5">
@@ -1773,8 +1773,8 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="3">
         <v>-4</v>
       </c>
@@ -1791,32 +1791,32 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1825,7 +1825,7 @@
       <c r="D14" s="2">
         <v>0.15915494309189501</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="26" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1834,7 +1834,7 @@
       <c r="H14" s="10">
         <v>2.2390899578253199E-17</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="26" t="s">
         <v>9</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1843,7 +1843,7 @@
       <c r="L14" s="2">
         <v>2.3927977920047E-4</v>
       </c>
-      <c r="N14" s="22" t="s">
+      <c r="N14" s="26" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -1854,28 +1854,28 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="8">
         <v>9.4387795134662607E-10</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="3">
         <v>7.9577471545947603E-2</v>
       </c>
-      <c r="J15" s="23"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="L15" s="8">
         <v>9.8206401731987101E-6</v>
       </c>
-      <c r="N15" s="23"/>
+      <c r="N15" s="27"/>
       <c r="O15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1884,7 +1884,7 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1894,7 +1894,7 @@
         <f>H5*D14</f>
         <v>0.1114084601643265</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="28" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1904,7 +1904,7 @@
         <f>H5*H14</f>
         <v>1.5673629704777237E-17</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="28" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1914,7 +1914,7 @@
         <f>L14*H5</f>
         <v>1.67495845440329E-4</v>
       </c>
-      <c r="N16" s="24" t="s">
+      <c r="N16" s="28" t="s">
         <v>12</v>
       </c>
       <c r="O16" s="2" t="s">
@@ -1926,15 +1926,15 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="20">
         <f>H7*D15</f>
         <v>2.8316338540398779E-10</v>
       </c>
-      <c r="F17" s="23"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1942,7 +1942,7 @@
         <f>H15*H7</f>
         <v>2.3873241463784282E-2</v>
       </c>
-      <c r="J17" s="23"/>
+      <c r="J17" s="27"/>
       <c r="K17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1950,7 +1950,7 @@
         <f>L15*H7</f>
         <v>2.9461920519596129E-6</v>
       </c>
-      <c r="N17" s="23"/>
+      <c r="N17" s="27"/>
       <c r="O17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1963,38 +1963,38 @@
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="30">
         <f>D16+D17</f>
         <v>0.11140846044748988</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="30"/>
       <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="31">
         <f>H16+H17</f>
         <v>2.3873241463784299E-2</v>
       </c>
-      <c r="H18" s="27"/>
+      <c r="H18" s="31"/>
       <c r="J18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="30">
         <f>L16+L17</f>
         <v>1.704420374922886E-4</v>
       </c>
-      <c r="L18" s="28"/>
+      <c r="L18" s="30"/>
       <c r="N18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="28">
+      <c r="O18" s="30">
         <f>P16+P17</f>
         <v>5.9020344217648163E-6</v>
       </c>
-      <c r="P18" s="28"/>
+      <c r="P18" s="30"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2004,7 +2004,7 @@
         <f>D16/C18</f>
         <v>0.99999999745833146</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="28" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -2014,29 +2014,29 @@
         <f>H16/G18</f>
         <v>6.5653546580819908E-16</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="21">
         <f>L16/K18</f>
         <v>0.98271440487741823</v>
       </c>
-      <c r="N19" s="24" t="s">
+      <c r="N19" s="28" t="s">
         <v>14</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P19" s="31">
+      <c r="P19" s="23">
         <f>P16/O18</f>
         <v>0.85698183117248028</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2044,7 +2044,7 @@
         <f>D17/C18</f>
         <v>2.5416685973993073E-9</v>
       </c>
-      <c r="F20" s="23"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2052,19 +2052,19 @@
         <f>H17/G18</f>
         <v>0.99999999999999922</v>
       </c>
-      <c r="J20" s="23"/>
+      <c r="J20" s="27"/>
       <c r="K20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="22">
         <f>L17/K18</f>
         <v>1.7285595122581827E-2</v>
       </c>
-      <c r="N20" s="23"/>
+      <c r="N20" s="27"/>
       <c r="O20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="30">
+      <c r="P20" s="22">
         <f>P17/O18</f>
         <v>0.14301816882751966</v>
       </c>
@@ -2073,35 +2073,35 @@
       <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="21" t="str">
+      <c r="C21" s="32" t="str">
         <f>IF(D19&gt;D20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="32"/>
       <c r="F21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="21" t="str">
+      <c r="G21" s="32" t="str">
         <f>IF(H19&gt;H20, "c1", "c2")</f>
         <v>c2</v>
       </c>
-      <c r="H21" s="21"/>
+      <c r="H21" s="32"/>
       <c r="J21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="21" t="str">
+      <c r="K21" s="32" t="str">
         <f>IF(L19&gt;L20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="L21" s="21"/>
+      <c r="L21" s="32"/>
       <c r="N21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="21" t="str">
+      <c r="O21" s="32" t="str">
         <f>IF(P19&gt;P20, "c1", "c2")</f>
         <v>c1</v>
       </c>
-      <c r="P21" s="21"/>
+      <c r="P21" s="32"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2144,10 +2144,10 @@
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
@@ -2228,11 +2228,11 @@
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="32">
+      <c r="B31" s="24">
         <f>SUM(B27:B30)</f>
         <v>2.8396962335082305</v>
       </c>
-      <c r="D31" s="33">
+      <c r="D31" s="25">
         <f>SUM(D27:D30)</f>
         <v>1.1603037664917693</v>
       </c>
@@ -2240,10 +2240,10 @@
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M33">
@@ -2282,10 +2282,10 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M36">
@@ -2324,10 +2324,10 @@
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M39">
@@ -2366,10 +2366,10 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M42">
@@ -2432,16 +2432,25 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="N19:N20"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B20"/>
@@ -2451,25 +2460,16 @@
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2481,34 +2481,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2303F90-97BD-41BC-954F-99D4AF5EB548}">
   <dimension ref="B4:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="G4" s="20" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="G4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="L4" s="25" t="s">
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="L4" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
@@ -2562,25 +2562,25 @@
         <v>4.0388436152317801</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>4.49535804129924</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4.9286503810670403</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
       </c>
       <c r="G6">
         <v>8.5440037453175304</v>
       </c>
       <c r="H6">
+        <v>6.9823759942501198</v>
+      </c>
+      <c r="I6">
         <v>6</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>6.4031242374328396</v>
-      </c>
-      <c r="J6">
-        <v>6.9823759942501198</v>
       </c>
       <c r="L6">
         <f xml:space="preserve"> 1 - B6/G6</f>
@@ -2588,27 +2588,27 @@
       </c>
       <c r="M6">
         <f xml:space="preserve"> 1 - C6/H6</f>
-        <v>0.25077365978346</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f xml:space="preserve"> 1 - D6/I6</f>
-        <v>0.2302741289550474</v>
+        <v>0.25077365978346</v>
       </c>
       <c r="O6">
         <f xml:space="preserve"> 1 - E6/J6</f>
-        <v>0.85678227571481613</v>
+        <v>0.2302741289550474</v>
       </c>
       <c r="P6">
         <f>(L6 + N6 + O6)/3</f>
-        <v>0.53811517153245614</v>
+        <v>0.33611229955533745</v>
       </c>
       <c r="Q6">
         <f>M6</f>
-        <v>0.25077365978346</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f>(P6 + Q6)/2</f>
-        <v>0.39444441565795807</v>
+        <v>0.6680561497776687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>